<commit_message>
Correct pie chart labels (forgot to add excel in last update).
</commit_message>
<xml_diff>
--- a/renders/Performance Analysis.xlsx
+++ b/renders/Performance Analysis.xlsx
@@ -425,304 +425,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="2.1099884037243063E-3"/>
-          <c:y val="2.5052197557728549E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>triangle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.14960114714933284"/>
-                  <c:y val="-2.9615730412929475E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US"/>
-                      <a:t>Vertex Shader
-</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US" sz="2000" b="1"/>
-                      <a:t>7%</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" altLang="en-US" b="1"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.27369729248790753"/>
-                  <c:y val="4.8625811347089321E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US"/>
-                      <a:t>Primitive Assembly
-</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US" sz="2000" b="1"/>
-                      <a:t>20%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.18331412403755418"/>
-                  <c:y val="-0.22578583461516713"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US"/>
-                      <a:t>Rasterization
-</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US" sz="2000" b="1"/>
-                      <a:t>21%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.1592352820885527"/>
-                  <c:y val="0.14283741671733363"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US"/>
-                      <a:t>Fragment Shader
-</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US" sz="2000" b="1"/>
-                      <a:t>33%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.9781881848779684E-2"/>
-                  <c:y val="1.6539053154056332E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US"/>
-                      <a:t>Fragments to Framebuffer
-</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="en-US" sz="2000" b="1"/>
-                      <a:t>19%</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" altLang="en-US" b="1"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200"/>
-                </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Vertex Shader</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Primitive Assembly</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Rasterization</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Fragment Shader</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Fragments to Framebuffer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>7.6830700000000003E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.72869E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1108E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0696299999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.9915999999999998E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="1"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId1"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -859,11 +561,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="113782272"/>
-        <c:axId val="115408896"/>
+        <c:axId val="141700608"/>
+        <c:axId val="142016512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113782272"/>
+        <c:axId val="141700608"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -889,7 +591,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115408896"/>
+        <c:crossAx val="142016512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -897,7 +599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115408896"/>
+        <c:axId val="142016512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,7 +646,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113782272"/>
+        <c:crossAx val="141700608"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0000000000000012E-4"/>
@@ -1005,6 +707,310 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.3200332502078135E-2"/>
+          <c:y val="2.2662887271665957E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>triangle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.25285965098957225"/>
+                  <c:y val="6.5170678646481748E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP"/>
+                      <a:t>Vertex Shader
+</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="2000" b="1"/>
+                      <a:t>1%</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" altLang="ja-JP" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.29064339930481664"/>
+                  <c:y val="0.15419297176980923"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP"/>
+                      <a:t>Primitive Assembly
+</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="2000" b="1"/>
+                      <a:t>1%</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" altLang="ja-JP" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.17660042916932681"/>
+                  <c:y val="-0.21598786837909476"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP"/>
+                      <a:t>Rasterization
+</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="2000" b="1"/>
+                      <a:t>72%</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" altLang="ja-JP" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17136101652833935"/>
+                  <c:y val="0.14451009559825873"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0"/>
+                      <a:t>Fragment Shader</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="1200"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="2000" b="1"/>
+                      <a:t>20%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.8718876356671635E-2"/>
+                  <c:y val="2.4113917426681071E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP"/>
+                      <a:t>Fragments to Framebuffer
+</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="ja-JP" sz="2000" b="1"/>
+                      <a:t>6%</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" altLang="ja-JP" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:endParaRPr lang="ja-JP"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Vertex Shader</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Primitive Assembly</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rasterization</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fragment Shader</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fragments to Framebuffer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>7.6830700000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.72869E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1108E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0696299999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9915999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1039,23 +1045,21 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1071,20 +1075,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1194,22 +1198,22 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.50168</cdr:x>
-      <cdr:y>0.13779</cdr:y>
+      <cdr:x>0.49887</cdr:x>
+      <cdr:y>0.13417</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.55724</cdr:x>
-      <cdr:y>0.13779</cdr:y>
+      <cdr:x>0.55462</cdr:x>
+      <cdr:y>0.13417</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <cdr:cNvPr id="2" name="Straight Arrow Connector 1"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2838452" y="628649"/>
-          <a:ext cx="314325" cy="0"/>
+          <a:off x="2813031" y="612788"/>
+          <a:ext cx="314350" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -1237,22 +1241,22 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.5</cdr:x>
-      <cdr:y>0.13361</cdr:y>
+      <cdr:x>0.49718</cdr:x>
+      <cdr:y>0.12999</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.5</cdr:x>
-      <cdr:y>0.54489</cdr:y>
+      <cdr:x>0.49718</cdr:x>
+      <cdr:y>0.54085</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="6" name="Straight Connector 5"/>
+        <cdr:cNvPr id="3" name="Straight Connector 2"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="2828927" y="609599"/>
-          <a:ext cx="0" cy="1876425"/>
+          <a:off x="2803526" y="593717"/>
+          <a:ext cx="0" cy="1876454"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -1567,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>